<commit_message>
Added reporting for field statistics
</commit_message>
<xml_diff>
--- a/doc/CDC_COVID-19_Vaccination_Reporting_Specification_with_HL7_Mapping.xlsx
+++ b/doc/CDC_COVID-19_Vaccination_Reporting_Specification_with_HL7_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kboone\git\CDC_IIS_Open_Tools\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14364005-ADA2-4DC5-B98E-D66BF0F9A131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C43BA9-4554-4C81-AC2A-EB86FE6DED16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="491" firstSheet="4" activeTab="4" xr2:uid="{345F94AC-3EB1-4843-98B7-0CF9FCF4D743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="348" firstSheet="4" activeTab="4" xr2:uid="{345F94AC-3EB1-4843-98B7-0CF9FCF4D743}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary Background" sheetId="28" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Categories!$A$4:$N$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CDC COVID-19 Vaccination Report'!$A$2:$I$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CDC COVID-19 Vaccination Report'!$A$2:$J$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ext. Data Sources'!$A$3:$F$40</definedName>
     <definedName name="_ftn1" localSheetId="3">Instructions!$A$19</definedName>
     <definedName name="_ftnref1" localSheetId="3">Instructions!$A$8</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="839">
   <si>
     <t>COVID-19 Vaccination IIS Data Dictionary</t>
   </si>
@@ -2866,6 +2866,42 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Minimally acceptable</t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>If pprl_id is valued, treat as if P, otherwise if recip_first_name = 'Redacted' treat as D, otherwise treat as I</t>
+  </si>
+  <si>
+    <t>Reject records where this field if populated until PPRL is available.</t>
+  </si>
+  <si>
+    <t>If YYYY-MM is valid but YYYY-MM-DD is not a valid date, accept as YYYY-MM.  If YYYY-MM is not valid, accept as if YYYY-01 was submitted.  At present, use cases for reporting from Data Lake are concerned with Age in years, rather than being more precise.</t>
+  </si>
+  <si>
+    <t>Treat as 'U', Unknown.</t>
+  </si>
+  <si>
+    <t>If invalid, treat as if not sent</t>
+  </si>
+  <si>
+    <t>If invalid, treat as if UNK.</t>
+  </si>
+  <si>
+    <t>If invalid, treat as 213 (COVID-19 Unspecified), which can be inferred from context.</t>
+  </si>
+  <si>
+    <t>If invalid, treat as if not present.</t>
+  </si>
+  <si>
+    <t>If not present and admin_name is present, use admin_name for responsible_org.</t>
+  </si>
+  <si>
+    <t>If not present and responsible_org is present, use responsible_org for admin_name.</t>
   </si>
 </sst>
 </file>
@@ -3547,7 +3583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3931,6 +3967,18 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3960,12 +4008,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6458,122 +6500,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
     </row>
     <row r="3" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="137"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
     </row>
     <row r="4" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="135" t="s">
+      <c r="A4" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
+      <c r="B4" s="142"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
     </row>
     <row r="5" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="139"/>
-      <c r="J5" s="139"/>
-      <c r="K5" s="139"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
     </row>
     <row r="6" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="140" t="s">
+      <c r="A6" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="140"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="140"/>
-      <c r="K6" s="140"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="144"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="144"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="144"/>
+      <c r="K6" s="144"/>
     </row>
     <row r="7" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="141" t="s">
+      <c r="A7" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="141"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
-      <c r="J7" s="141"/>
-      <c r="K7" s="141"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
     </row>
     <row r="8" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
-      <c r="K8" s="135"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0"/>
@@ -7750,11 +7792,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9023E05B-6C0B-495B-B56F-D7589B512959}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="A1:I1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7763,37 +7805,38 @@
     <col min="2" max="3" width="35.42578125" style="89" customWidth="1"/>
     <col min="4" max="4" width="59.85546875" style="89" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" style="89" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" style="89" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" style="89" customWidth="1"/>
-    <col min="8" max="9" width="35.42578125" style="89" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33" customWidth="1"/>
+    <col min="6" max="7" width="49.42578125" style="89" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" style="89" customWidth="1"/>
+    <col min="9" max="10" width="35.42578125" style="89" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="40.7109375" customWidth="1"/>
+    <col min="13" max="13" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="90" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="142" t="s">
+    <row r="1" spans="1:13" s="90" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="142" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="146" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143" t="s">
+      <c r="F1" s="147"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="147" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="143"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="133" t="s">
+      <c r="I1" s="147"/>
+      <c r="J1" s="148"/>
+      <c r="K1" s="133" t="s">
         <v>743</v>
       </c>
-      <c r="K1" s="133"/>
-      <c r="L1" s="134"/>
-    </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L1" s="133"/>
+      <c r="M1" s="134"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
         <v>164</v>
       </c>
@@ -7813,25 +7856,28 @@
         <v>169</v>
       </c>
       <c r="G2" s="100" t="s">
+        <v>827</v>
+      </c>
+      <c r="H2" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="92" t="s">
+      <c r="I2" s="92" t="s">
         <v>171</v>
       </c>
-      <c r="I2" s="92" t="s">
+      <c r="J2" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="145" t="s">
+      <c r="K2" s="136" t="s">
         <v>744</v>
       </c>
-      <c r="K2" s="145" t="s">
+      <c r="L2" s="136" t="s">
         <v>745</v>
       </c>
-      <c r="L2" s="145" t="s">
+      <c r="M2" s="136" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="122">
         <v>1</v>
       </c>
@@ -7850,26 +7896,29 @@
       <c r="F3" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H3" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H3" s="104" t="s">
+      <c r="I3" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I3" s="97">
+      <c r="J3" s="97">
         <v>568971356</v>
       </c>
-      <c r="J3" s="146" t="s">
+      <c r="K3" s="137" t="s">
         <v>753</v>
       </c>
-      <c r="K3" s="146" t="s">
+      <c r="L3" s="137" t="s">
         <v>754</v>
       </c>
-      <c r="L3" s="146" t="s">
+      <c r="M3" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="90" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="90" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="122">
         <v>2</v>
       </c>
@@ -7888,26 +7937,29 @@
       <c r="F4" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="129" t="s">
+        <v>829</v>
+      </c>
+      <c r="H4" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="104" t="s">
+      <c r="I4" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="94" t="s">
+      <c r="J4" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="J4" s="146" t="s">
+      <c r="K4" s="137" t="s">
         <v>755</v>
       </c>
-      <c r="K4" s="146" t="s">
+      <c r="L4" s="137" t="s">
         <v>756</v>
       </c>
-      <c r="L4" s="146" t="s">
+      <c r="M4" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="90" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="90" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="122">
         <v>3</v>
       </c>
@@ -7926,24 +7978,27 @@
       <c r="F5" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="G5" s="117" t="s">
+      <c r="G5" s="129" t="s">
+        <v>830</v>
+      </c>
+      <c r="H5" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H5" s="104" t="s">
+      <c r="I5" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="146" t="s">
+      <c r="J5" s="94"/>
+      <c r="K5" s="137" t="s">
         <v>757</v>
       </c>
-      <c r="K5" s="146" t="s">
+      <c r="L5" s="137" t="s">
         <v>758</v>
       </c>
-      <c r="L5" s="146" t="s">
+      <c r="M5" s="137" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="122">
         <v>4</v>
       </c>
@@ -7962,26 +8017,29 @@
       <c r="F6" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G6" s="117" t="s">
+      <c r="G6" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H6" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H6" s="104" t="s">
+      <c r="I6" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="94">
+      <c r="J6" s="94">
         <v>135498413</v>
       </c>
-      <c r="J6" s="146" t="s">
+      <c r="K6" s="137" t="s">
         <v>760</v>
       </c>
-      <c r="K6" s="146" t="s">
+      <c r="L6" s="137" t="s">
         <v>758</v>
       </c>
-      <c r="L6" s="146" t="s">
+      <c r="M6" s="137" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="122">
         <v>5</v>
       </c>
@@ -8000,26 +8058,29 @@
       <c r="F7" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G7" s="117" t="s">
+      <c r="G7" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H7" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H7" s="104" t="s">
+      <c r="I7" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I7" s="94" t="s">
+      <c r="J7" s="94" t="s">
         <v>197</v>
       </c>
-      <c r="J7" s="146" t="s">
+      <c r="K7" s="137" t="s">
         <v>761</v>
       </c>
-      <c r="K7" s="146" t="s">
+      <c r="L7" s="137" t="s">
         <v>762</v>
       </c>
-      <c r="L7" s="146" t="s">
+      <c r="M7" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="122">
         <v>6</v>
       </c>
@@ -8038,26 +8099,29 @@
       <c r="F8" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H8" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H8" s="104" t="s">
+      <c r="I8" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I8" s="94" t="s">
+      <c r="J8" s="94" t="s">
         <v>197</v>
       </c>
-      <c r="J8" s="146" t="s">
+      <c r="K8" s="137" t="s">
         <v>763</v>
       </c>
-      <c r="K8" s="146" t="s">
+      <c r="L8" s="137" t="s">
         <v>764</v>
       </c>
-      <c r="L8" s="146" t="s">
+      <c r="M8" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="122">
         <v>7</v>
       </c>
@@ -8076,26 +8140,29 @@
       <c r="F9" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="117" t="s">
+      <c r="G9" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H9" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H9" s="104" t="s">
+      <c r="I9" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I9" s="94" t="s">
+      <c r="J9" s="94" t="s">
         <v>197</v>
       </c>
-      <c r="J9" s="146" t="s">
+      <c r="K9" s="137" t="s">
         <v>765</v>
       </c>
-      <c r="K9" s="146" t="s">
+      <c r="L9" s="137" t="s">
         <v>766</v>
       </c>
-      <c r="L9" s="146" t="s">
+      <c r="M9" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="122">
         <v>8</v>
       </c>
@@ -8114,26 +8181,29 @@
       <c r="F10" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="129" t="s">
+        <v>831</v>
+      </c>
+      <c r="H10" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H10" s="95" t="s">
+      <c r="I10" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="I10" s="128">
+      <c r="J10" s="128">
         <v>24985</v>
       </c>
-      <c r="J10" s="146" t="s">
+      <c r="K10" s="137" t="s">
         <v>767</v>
       </c>
-      <c r="K10" s="146" t="s">
+      <c r="L10" s="137" t="s">
         <v>768</v>
       </c>
-      <c r="L10" s="146" t="s">
+      <c r="M10" s="137" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="122">
         <v>9</v>
       </c>
@@ -8153,25 +8223,28 @@
         <v>176</v>
       </c>
       <c r="G11" s="129" t="s">
+        <v>832</v>
+      </c>
+      <c r="H11" s="129" t="s">
         <v>211</v>
       </c>
-      <c r="H11" s="104" t="s">
+      <c r="I11" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="J11" s="97" t="s">
         <v>212</v>
       </c>
-      <c r="J11" s="146" t="s">
+      <c r="K11" s="137" t="s">
         <v>770</v>
       </c>
-      <c r="K11" s="146" t="s">
+      <c r="L11" s="137" t="s">
         <v>771</v>
       </c>
-      <c r="L11" s="146" t="s">
+      <c r="M11" s="137" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="122">
         <v>10</v>
       </c>
@@ -8190,26 +8263,29 @@
       <c r="F12" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G12" s="117" t="s">
+      <c r="G12" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H12" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H12" s="104" t="s">
+      <c r="I12" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="J12" s="97" t="s">
         <v>197</v>
       </c>
-      <c r="J12" s="146" t="s">
+      <c r="K12" s="137" t="s">
         <v>773</v>
       </c>
-      <c r="K12" s="146" t="s">
+      <c r="L12" s="137" t="s">
         <v>774</v>
       </c>
-      <c r="L12" s="146" t="s">
+      <c r="M12" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="90" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="90" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="122">
         <v>11</v>
       </c>
@@ -8228,26 +8304,29 @@
       <c r="F13" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G13" s="117" t="s">
+      <c r="G13" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H13" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H13" s="104" t="s">
+      <c r="I13" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I13" s="97" t="s">
+      <c r="J13" s="97" t="s">
         <v>197</v>
       </c>
-      <c r="J13" s="146" t="s">
+      <c r="K13" s="137" t="s">
         <v>775</v>
       </c>
-      <c r="K13" s="146" t="s">
+      <c r="L13" s="137" t="s">
         <v>776</v>
       </c>
-      <c r="L13" s="146" t="s">
+      <c r="M13" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="122">
         <v>12</v>
       </c>
@@ -8266,26 +8345,29 @@
       <c r="F14" s="98" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="117" t="s">
+      <c r="G14" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H14" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H14" s="104" t="s">
+      <c r="I14" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I14" s="97" t="s">
+      <c r="J14" s="97" t="s">
         <v>197</v>
       </c>
-      <c r="J14" s="146" t="s">
+      <c r="K14" s="137" t="s">
         <v>777</v>
       </c>
-      <c r="K14" s="146" t="s">
+      <c r="L14" s="137" t="s">
         <v>778</v>
       </c>
-      <c r="L14" s="146" t="s">
+      <c r="M14" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="122">
         <v>13</v>
       </c>
@@ -8304,26 +8386,29 @@
       <c r="F15" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="G15" s="117" t="s">
+      <c r="G15" s="129" t="s">
+        <v>833</v>
+      </c>
+      <c r="H15" s="117" t="s">
         <v>226</v>
       </c>
-      <c r="H15" s="104" t="s">
+      <c r="I15" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I15" s="97">
+      <c r="J15" s="97">
         <v>13121</v>
       </c>
-      <c r="J15" s="146" t="s">
+      <c r="K15" s="137" t="s">
         <v>779</v>
       </c>
-      <c r="K15" s="146" t="s">
+      <c r="L15" s="137" t="s">
         <v>780</v>
       </c>
-      <c r="L15" s="146" t="s">
+      <c r="M15" s="137" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="122">
         <v>14</v>
       </c>
@@ -8342,26 +8427,29 @@
       <c r="F16" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="117" t="s">
+      <c r="G16" s="129" t="s">
+        <v>833</v>
+      </c>
+      <c r="H16" s="117" t="s">
         <v>230</v>
       </c>
-      <c r="H16" s="104" t="s">
+      <c r="I16" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I16" s="97" t="s">
+      <c r="J16" s="97" t="s">
         <v>231</v>
       </c>
-      <c r="J16" s="146" t="s">
+      <c r="K16" s="137" t="s">
         <v>781</v>
       </c>
-      <c r="K16" s="146" t="s">
+      <c r="L16" s="137" t="s">
         <v>782</v>
       </c>
-      <c r="L16" s="146" t="s">
+      <c r="M16" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="122">
         <v>15</v>
       </c>
@@ -8380,26 +8468,29 @@
       <c r="F17" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="G17" s="117" t="s">
+      <c r="G17" s="129" t="s">
+        <v>833</v>
+      </c>
+      <c r="H17" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H17" s="104" t="s">
+      <c r="I17" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I17" s="97">
+      <c r="J17" s="97">
         <v>30301</v>
       </c>
-      <c r="J17" s="146" t="s">
+      <c r="K17" s="137" t="s">
         <v>783</v>
       </c>
-      <c r="K17" s="146" t="s">
+      <c r="L17" s="137" t="s">
         <v>784</v>
       </c>
-      <c r="L17" s="146" t="s">
+      <c r="M17" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A18" s="122">
         <v>16</v>
       </c>
@@ -8419,25 +8510,28 @@
         <v>176</v>
       </c>
       <c r="G18" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H18" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="I18" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I18" s="94" t="s">
+      <c r="J18" s="94" t="s">
         <v>239</v>
       </c>
-      <c r="J18" s="146" t="s">
+      <c r="K18" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K18" s="146" t="s">
+      <c r="L18" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L18" s="146" t="s">
+      <c r="M18" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="122">
         <v>17</v>
       </c>
@@ -8457,25 +8551,28 @@
         <v>225</v>
       </c>
       <c r="G19" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H19" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="H19" s="104" t="s">
+      <c r="I19" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I19" s="94" t="s">
+      <c r="J19" s="94" t="s">
         <v>244</v>
       </c>
-      <c r="J19" s="146" t="s">
+      <c r="K19" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K19" s="146" t="s">
+      <c r="L19" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L19" s="146" t="s">
+      <c r="M19" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="122">
         <v>18</v>
       </c>
@@ -8495,25 +8592,28 @@
         <v>225</v>
       </c>
       <c r="G20" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H20" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="H20" s="104" t="s">
+      <c r="I20" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I20" s="94" t="s">
+      <c r="J20" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="J20" s="146" t="s">
+      <c r="K20" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K20" s="146" t="s">
+      <c r="L20" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L20" s="146" t="s">
+      <c r="M20" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="122">
         <v>19</v>
       </c>
@@ -8533,25 +8633,28 @@
         <v>225</v>
       </c>
       <c r="G21" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H21" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="H21" s="104" t="s">
+      <c r="I21" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I21" s="94" t="s">
+      <c r="J21" s="94" t="s">
         <v>250</v>
       </c>
-      <c r="J21" s="146" t="s">
+      <c r="K21" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K21" s="146" t="s">
+      <c r="L21" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L21" s="146" t="s">
+      <c r="M21" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="122">
         <v>20</v>
       </c>
@@ -8571,25 +8674,28 @@
         <v>225</v>
       </c>
       <c r="G22" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H22" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="H22" s="104" t="s">
+      <c r="I22" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I22" s="94" t="s">
+      <c r="J22" s="94" t="s">
         <v>253</v>
       </c>
-      <c r="J22" s="146" t="s">
+      <c r="K22" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K22" s="146" t="s">
+      <c r="L22" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L22" s="146" t="s">
+      <c r="M22" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="122">
         <v>21</v>
       </c>
@@ -8609,25 +8715,28 @@
         <v>225</v>
       </c>
       <c r="G23" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H23" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="H23" s="104" t="s">
+      <c r="I23" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I23" s="94" t="s">
+      <c r="J23" s="94" t="s">
         <v>256</v>
       </c>
-      <c r="J23" s="146" t="s">
+      <c r="K23" s="137" t="s">
         <v>785</v>
       </c>
-      <c r="K23" s="146" t="s">
+      <c r="L23" s="137" t="s">
         <v>786</v>
       </c>
-      <c r="L23" s="146" t="s">
+      <c r="M23" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A24" s="122">
         <v>22</v>
       </c>
@@ -8646,26 +8755,29 @@
       <c r="F24" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="117" t="s">
+      <c r="G24" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H24" s="117" t="s">
         <v>260</v>
       </c>
-      <c r="H24" s="104" t="s">
+      <c r="I24" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I24" s="94" t="s">
+      <c r="J24" s="94" t="s">
         <v>261</v>
       </c>
-      <c r="J24" s="146" t="s">
+      <c r="K24" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="K24" s="146" t="s">
+      <c r="L24" s="137" t="s">
         <v>788</v>
       </c>
-      <c r="L24" s="146" t="s">
+      <c r="M24" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="122">
         <v>23</v>
       </c>
@@ -8684,26 +8796,29 @@
       <c r="F25" s="98" t="s">
         <v>265</v>
       </c>
-      <c r="G25" s="117" t="s">
+      <c r="G25" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H25" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H25" s="95" t="s">
+      <c r="I25" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="I25" s="128">
+      <c r="J25" s="128">
         <v>44180</v>
       </c>
-      <c r="J25" s="146" t="s">
+      <c r="K25" s="137" t="s">
         <v>789</v>
       </c>
-      <c r="K25" s="146" t="s">
+      <c r="L25" s="137" t="s">
         <v>790</v>
       </c>
-      <c r="L25" s="146" t="s">
+      <c r="M25" s="137" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="126" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="126" x14ac:dyDescent="0.25">
       <c r="A26" s="122">
         <v>24</v>
       </c>
@@ -8723,25 +8838,28 @@
         <v>176</v>
       </c>
       <c r="G26" s="129" t="s">
+        <v>835</v>
+      </c>
+      <c r="H26" s="129" t="s">
         <v>269</v>
       </c>
-      <c r="H26" s="104" t="s">
+      <c r="I26" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I26" s="96" t="s">
+      <c r="J26" s="96" t="s">
         <v>270</v>
       </c>
-      <c r="J26" s="146" t="s">
+      <c r="K26" s="137" t="s">
         <v>791</v>
       </c>
-      <c r="K26" s="146" t="s">
+      <c r="L26" s="137" t="s">
         <v>792</v>
       </c>
-      <c r="L26" s="146" t="s">
+      <c r="M26" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="90" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="90" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="122">
         <v>25</v>
       </c>
@@ -8761,23 +8879,26 @@
         <v>189</v>
       </c>
       <c r="G27" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H27" s="129" t="s">
         <v>275</v>
       </c>
-      <c r="H27" s="104" t="s">
+      <c r="I27" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I27" s="96"/>
-      <c r="J27" s="146" t="s">
+      <c r="J27" s="96"/>
+      <c r="K27" s="137" t="s">
         <v>793</v>
       </c>
-      <c r="K27" s="146" t="s">
+      <c r="L27" s="137" t="s">
         <v>792</v>
       </c>
-      <c r="L27" s="146" t="s">
+      <c r="M27" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A28" s="122">
         <v>26</v>
       </c>
@@ -8797,25 +8918,28 @@
         <v>189</v>
       </c>
       <c r="G28" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H28" s="129" t="s">
         <v>279</v>
       </c>
-      <c r="H28" s="104" t="s">
+      <c r="I28" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I28" s="94" t="s">
+      <c r="J28" s="94" t="s">
         <v>280</v>
       </c>
-      <c r="J28" s="146" t="s">
+      <c r="K28" s="137" t="s">
         <v>794</v>
       </c>
-      <c r="K28" s="146" t="s">
+      <c r="L28" s="137" t="s">
         <v>795</v>
       </c>
-      <c r="L28" s="146" t="s">
+      <c r="M28" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="122">
         <v>27</v>
       </c>
@@ -8834,26 +8958,29 @@
       <c r="F29" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="G29" s="117" t="s">
+      <c r="G29" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H29" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H29" s="104" t="s">
+      <c r="I29" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I29" s="97" t="s">
+      <c r="J29" s="97" t="s">
         <v>284</v>
       </c>
-      <c r="J29" s="146" t="s">
+      <c r="K29" s="137" t="s">
         <v>796</v>
       </c>
-      <c r="K29" s="146" t="s">
+      <c r="L29" s="137" t="s">
         <v>797</v>
       </c>
-      <c r="L29" s="146" t="s">
+      <c r="M29" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="90" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="90" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="122">
         <v>28</v>
       </c>
@@ -8872,26 +8999,29 @@
       <c r="F30" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="G30" s="117" t="s">
+      <c r="G30" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H30" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H30" s="95" t="s">
+      <c r="I30" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="I30" s="128">
+      <c r="J30" s="128">
         <v>44365</v>
       </c>
-      <c r="J30" s="146" t="s">
+      <c r="K30" s="137" t="s">
         <v>798</v>
       </c>
-      <c r="K30" s="146" t="s">
+      <c r="L30" s="137" t="s">
         <v>799</v>
       </c>
-      <c r="L30" s="146" t="s">
+      <c r="M30" s="137" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="90" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="90" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A31" s="122">
         <v>29</v>
       </c>
@@ -8911,25 +9041,28 @@
         <v>189</v>
       </c>
       <c r="G31" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H31" s="129" t="s">
         <v>291</v>
       </c>
-      <c r="H31" s="104" t="s">
+      <c r="I31" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I31" s="97" t="s">
+      <c r="J31" s="97" t="s">
         <v>292</v>
       </c>
-      <c r="J31" s="146" t="s">
+      <c r="K31" s="137" t="s">
         <v>800</v>
       </c>
-      <c r="K31" s="146" t="s">
+      <c r="L31" s="137" t="s">
         <v>801</v>
       </c>
-      <c r="L31" s="146" t="s">
+      <c r="M31" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="90" customFormat="1" ht="189" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="90" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A32" s="122">
         <v>30</v>
       </c>
@@ -8948,26 +9081,29 @@
       <c r="F32" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="G32" s="101" t="s">
+      <c r="G32" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H32" s="101" t="s">
         <v>296</v>
       </c>
-      <c r="H32" s="104" t="s">
+      <c r="I32" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I32" s="97" t="s">
+      <c r="J32" s="97" t="s">
         <v>297</v>
       </c>
-      <c r="J32" s="146" t="s">
+      <c r="K32" s="137" t="s">
         <v>802</v>
       </c>
-      <c r="K32" s="146" t="s">
+      <c r="L32" s="137" t="s">
         <v>803</v>
       </c>
-      <c r="L32" s="146" t="s">
+      <c r="M32" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="90" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="90" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A33" s="122">
         <v>31</v>
       </c>
@@ -8986,26 +9122,29 @@
       <c r="F33" s="98" t="s">
         <v>189</v>
       </c>
-      <c r="G33" s="101" t="s">
+      <c r="G33" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H33" s="101" t="s">
         <v>301</v>
       </c>
-      <c r="H33" s="104" t="s">
+      <c r="I33" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I33" s="94">
+      <c r="J33" s="94">
         <v>2</v>
       </c>
-      <c r="J33" s="146" t="s">
+      <c r="K33" s="137" t="s">
         <v>747</v>
       </c>
-      <c r="K33" s="146" t="s">
+      <c r="L33" s="137" t="s">
         <v>748</v>
       </c>
-      <c r="L33" s="146" t="s">
+      <c r="M33" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="90" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="90" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34" s="122">
         <v>32</v>
       </c>
@@ -9025,25 +9164,28 @@
         <v>189</v>
       </c>
       <c r="G34" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H34" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H34" s="104" t="s">
+      <c r="I34" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I34" s="97" t="s">
+      <c r="J34" s="97" t="s">
         <v>306</v>
       </c>
-      <c r="J34" s="146" t="s">
+      <c r="K34" s="137" t="s">
         <v>750</v>
       </c>
-      <c r="K34" s="146" t="s">
+      <c r="L34" s="137" t="s">
         <v>748</v>
       </c>
-      <c r="L34" s="146" t="s">
+      <c r="M34" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="90" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="90" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A35" s="122">
         <v>33</v>
       </c>
@@ -9062,26 +9204,29 @@
       <c r="F35" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G35" s="117" t="s">
+      <c r="G35" s="129" t="s">
+        <v>837</v>
+      </c>
+      <c r="H35" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H35" s="104" t="s">
+      <c r="I35" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I35" s="97" t="s">
+      <c r="J35" s="97" t="s">
         <v>310</v>
       </c>
-      <c r="J35" s="146" t="s">
+      <c r="K35" s="137" t="s">
         <v>804</v>
       </c>
-      <c r="K35" s="146" t="s">
+      <c r="L35" s="137" t="s">
         <v>805</v>
       </c>
-      <c r="L35" s="146" t="s">
+      <c r="M35" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="122">
         <v>34</v>
       </c>
@@ -9100,26 +9245,29 @@
       <c r="F36" s="126" t="s">
         <v>176</v>
       </c>
-      <c r="G36" s="117" t="s">
+      <c r="G36" s="129" t="s">
+        <v>838</v>
+      </c>
+      <c r="H36" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H36" s="104" t="s">
+      <c r="I36" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I36" s="94" t="s">
+      <c r="J36" s="94" t="s">
         <v>314</v>
       </c>
-      <c r="J36" s="146" t="s">
+      <c r="K36" s="137" t="s">
         <v>806</v>
       </c>
-      <c r="K36" s="146" t="s">
+      <c r="L36" s="137" t="s">
         <v>807</v>
       </c>
-      <c r="L36" s="146" t="s">
+      <c r="M36" s="137" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="90" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="90" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A37" s="122">
         <v>35</v>
       </c>
@@ -9138,26 +9286,29 @@
       <c r="F37" s="126" t="s">
         <v>274</v>
       </c>
-      <c r="G37" s="117" t="s">
+      <c r="G37" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H37" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H37" s="104" t="s">
+      <c r="I37" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I37" s="94">
+      <c r="J37" s="94">
         <v>123456</v>
       </c>
-      <c r="J37" s="146" t="s">
+      <c r="K37" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="K37" s="146" t="s">
+      <c r="L37" s="137" t="s">
         <v>809</v>
       </c>
-      <c r="L37" s="146" t="s">
+      <c r="M37" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" s="122">
         <v>36</v>
       </c>
@@ -9176,26 +9327,29 @@
       <c r="F38" s="98" t="s">
         <v>176</v>
       </c>
-      <c r="G38" s="117" t="s">
+      <c r="G38" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H38" s="117" t="s">
         <v>321</v>
       </c>
-      <c r="H38" s="104" t="s">
+      <c r="I38" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I38" s="94">
+      <c r="J38" s="94">
         <v>17</v>
       </c>
-      <c r="J38" s="146" t="s">
+      <c r="K38" s="137" t="s">
         <v>810</v>
       </c>
-      <c r="K38" s="146" t="s">
+      <c r="L38" s="137" t="s">
         <v>811</v>
       </c>
-      <c r="L38" s="146" t="s">
+      <c r="M38" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A39" s="122">
         <v>37</v>
       </c>
@@ -9214,26 +9368,29 @@
       <c r="F39" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G39" s="117" t="s">
+      <c r="G39" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H39" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H39" s="104" t="s">
+      <c r="I39" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I39" s="94" t="s">
+      <c r="J39" s="94" t="s">
         <v>326</v>
       </c>
-      <c r="J39" s="146" t="s">
+      <c r="K39" s="137" t="s">
         <v>812</v>
       </c>
-      <c r="K39" s="146" t="s">
+      <c r="L39" s="137" t="s">
         <v>813</v>
       </c>
-      <c r="L39" s="146" t="s">
+      <c r="M39" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="90" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="90" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A40" s="122">
         <v>38</v>
       </c>
@@ -9252,26 +9409,29 @@
       <c r="F40" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G40" s="117" t="s">
+      <c r="G40" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H40" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H40" s="104" t="s">
+      <c r="I40" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I40" s="94" t="s">
+      <c r="J40" s="94" t="s">
         <v>330</v>
       </c>
-      <c r="J40" s="146" t="s">
+      <c r="K40" s="137" t="s">
         <v>814</v>
       </c>
-      <c r="K40" s="146" t="s">
+      <c r="L40" s="137" t="s">
         <v>815</v>
       </c>
-      <c r="L40" s="146" t="s">
+      <c r="M40" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A41" s="122">
         <v>39</v>
       </c>
@@ -9290,26 +9450,29 @@
       <c r="F41" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G41" s="117" t="s">
+      <c r="G41" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H41" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H41" s="104" t="s">
+      <c r="I41" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I41" s="94" t="s">
+      <c r="J41" s="94" t="s">
         <v>334</v>
       </c>
-      <c r="J41" s="146" t="s">
+      <c r="K41" s="137" t="s">
         <v>816</v>
       </c>
-      <c r="K41" s="146" t="s">
+      <c r="L41" s="137" t="s">
         <v>817</v>
       </c>
-      <c r="L41" s="146" t="s">
+      <c r="M41" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A42" s="122">
         <v>40</v>
       </c>
@@ -9328,26 +9491,29 @@
       <c r="F42" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G42" s="117" t="s">
+      <c r="G42" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H42" s="117" t="s">
         <v>338</v>
       </c>
-      <c r="H42" s="104" t="s">
+      <c r="I42" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I42" s="97">
+      <c r="J42" s="97">
         <v>13121</v>
       </c>
-      <c r="J42" s="146" t="s">
+      <c r="K42" s="137" t="s">
         <v>818</v>
       </c>
-      <c r="K42" s="146" t="s">
+      <c r="L42" s="137" t="s">
         <v>819</v>
       </c>
-      <c r="L42" s="146" t="s">
+      <c r="M42" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A43" s="122">
         <v>41</v>
       </c>
@@ -9366,26 +9532,29 @@
       <c r="F43" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G43" s="117" t="s">
+      <c r="G43" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H43" s="117" t="s">
         <v>342</v>
       </c>
-      <c r="H43" s="104" t="s">
+      <c r="I43" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="I43" s="97" t="s">
+      <c r="J43" s="97" t="s">
         <v>231</v>
       </c>
-      <c r="J43" s="146" t="s">
+      <c r="K43" s="137" t="s">
         <v>820</v>
       </c>
-      <c r="K43" s="146" t="s">
+      <c r="L43" s="137" t="s">
         <v>821</v>
       </c>
-      <c r="L43" s="146" t="s">
+      <c r="M43" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A44" s="122">
         <v>42</v>
       </c>
@@ -9404,26 +9573,29 @@
       <c r="F44" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G44" s="117" t="s">
+      <c r="G44" s="129" t="s">
+        <v>836</v>
+      </c>
+      <c r="H44" s="117" t="s">
         <v>177</v>
       </c>
-      <c r="H44" s="104" t="s">
+      <c r="I44" s="104" t="s">
         <v>178</v>
       </c>
-      <c r="I44" s="94">
+      <c r="J44" s="94">
         <v>30301</v>
       </c>
-      <c r="J44" s="146" t="s">
+      <c r="K44" s="137" t="s">
         <v>822</v>
       </c>
-      <c r="K44" s="146" t="s">
+      <c r="L44" s="137" t="s">
         <v>823</v>
       </c>
-      <c r="L44" s="146" t="s">
+      <c r="M44" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A45" s="122">
         <v>43</v>
       </c>
@@ -9443,25 +9615,28 @@
         <v>350</v>
       </c>
       <c r="G45" s="129" t="s">
+        <v>828</v>
+      </c>
+      <c r="H45" s="129" t="s">
         <v>351</v>
       </c>
-      <c r="H45" s="98" t="s">
+      <c r="I45" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="I45" s="94" t="s">
+      <c r="J45" s="94" t="s">
         <v>352</v>
       </c>
-      <c r="J45" s="146" t="s">
+      <c r="K45" s="137" t="s">
         <v>824</v>
       </c>
-      <c r="K45" s="146" t="s">
+      <c r="L45" s="137" t="s">
         <v>825</v>
       </c>
-      <c r="L45" s="146" t="s">
+      <c r="M45" s="137" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A46" s="122">
         <v>44</v>
       </c>
@@ -9481,25 +9656,28 @@
         <v>176</v>
       </c>
       <c r="G46" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H46" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H46" s="98" t="s">
+      <c r="I46" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="I46" s="98" t="s">
+      <c r="J46" s="98" t="s">
         <v>306</v>
       </c>
-      <c r="J46" s="146" t="s">
+      <c r="K46" s="137" t="s">
         <v>751</v>
       </c>
-      <c r="K46" s="146" t="s">
+      <c r="L46" s="137" t="s">
         <v>748</v>
       </c>
-      <c r="L46" s="146" t="s">
+      <c r="M46" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A47" s="122">
         <v>45</v>
       </c>
@@ -9519,39 +9697,43 @@
         <v>176</v>
       </c>
       <c r="G47" s="129" t="s">
+        <v>834</v>
+      </c>
+      <c r="H47" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H47" s="98" t="s">
+      <c r="I47" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="I47" s="98" t="s">
+      <c r="J47" s="98" t="s">
         <v>359</v>
       </c>
-      <c r="J47" s="146" t="s">
+      <c r="K47" s="137" t="s">
         <v>752</v>
       </c>
-      <c r="K47" s="146" t="s">
+      <c r="L47" s="137" t="s">
         <v>748</v>
       </c>
-      <c r="L47" s="146" t="s">
+      <c r="M47" s="137" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="93"/>
       <c r="E48" s="103"/>
       <c r="F48" s="103"/>
-      <c r="J48" s="90"/>
+      <c r="G48" s="138"/>
+      <c r="K48" s="90"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I47" xr:uid="{6B127860-CA54-404E-9FCE-03790E862F86}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:I44">
+  <autoFilter ref="A2:J47" xr:uid="{6B127860-CA54-404E-9FCE-03790E862F86}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:J44">
     <sortCondition ref="B6:B44"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>